<commit_message>
updated all the xlsx sheets
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/biometric_attribute.xlsx
+++ b/mosip_master/xlsx/biometric_attribute.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop_Branch_all\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FCA8A4-11FA-4900-84B6-398AF1B490A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +171,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,16 +222,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,337 +507,338 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="1"/>
+    <col min="1" max="2" width="8.453125" style="2"/>
+    <col min="3" max="3" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated and uploading all new xlsx files to mosip data
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/biometric_attribute.xlsx
+++ b/mosip_master/xlsx/biometric_attribute.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop_Branch_all\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FCA8A4-11FA-4900-84B6-398AF1B490A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +171,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,16 +222,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,337 +507,338 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="1"/>
+    <col min="1" max="2" width="8.453125" style="2"/>
+    <col min="3" max="3" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>